<commit_message>
Atualização das planilhas - JULHO
</commit_message>
<xml_diff>
--- a/planilhas/RURAL/MODELO.xlsx
+++ b/planilhas/RURAL/MODELO.xlsx
@@ -328,8 +328,8 @@
   </sheetPr>
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:G179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>